<commit_message>
testdata excelsheet and newticket is updated
</commit_message>
<xml_diff>
--- a/Saran/src/main/resources/testdatalogin.xlsx
+++ b/Saran/src/main/resources/testdatalogin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neethu\eclipse-workspace-seleniumtraining\Saran\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neethu\git\Saran\Saran\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506039E-F51B-4B4B-8501-030A8371179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E77EB4-818F-445C-B34E-C984EFCEF749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{A5AB21CB-C963-41A1-8CA1-4E0096A38FDD}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="159">
   <si>
     <t>Username</t>
   </si>
@@ -511,6 +511,27 @@
   </si>
   <si>
     <t>teamdropdown</t>
+  </si>
+  <si>
+    <t>escalatedtoregion</t>
+  </si>
+  <si>
+    <t>escalatedtolocation</t>
+  </si>
+  <si>
+    <t>reasonforoccurrence</t>
+  </si>
+  <si>
+    <t>NERTCC</t>
+  </si>
+  <si>
+    <t>AIZWAL</t>
+  </si>
+  <si>
+    <t>Attenuator</t>
+  </si>
+  <si>
+    <t>subreasonoccurrence</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AC4E1D-DEF7-40CA-B4FC-DEED434DA9FE}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" activeCellId="1" sqref="Q1:Q1048576 P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A6659F-7721-4EC1-BAE0-E6CEED4F0246}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,9 +1936,17 @@
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" customWidth="1"/>
     <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="33.28515625" customWidth="1"/>
+    <col min="12" max="12" width="28" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1942,8 +1971,38 @@
       <c r="H1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1968,10 +2027,46 @@
       <c r="H2" t="s">
         <v>33</v>
       </c>
+      <c r="I2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2">
+        <v>91992345867</v>
+      </c>
+      <c r="P2">
+        <v>4712358669</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{A585FE40-9DBE-4591-A801-E7FFDE9DCD18}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changed in createuser of testdata excel
</commit_message>
<xml_diff>
--- a/Saran/src/main/resources/testdatalogin.xlsx
+++ b/Saran/src/main/resources/testdatalogin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neethu\git\Saran\Saran\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3132E475-0E48-4955-A4BF-D0BAFC03A67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69500C09-A955-4EB9-8F58-0B5D4A8618E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="12" xr2:uid="{A5AB21CB-C963-41A1-8CA1-4E0096A38FDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A5AB21CB-C963-41A1-8CA1-4E0096A38FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="163">
   <si>
     <t>Username</t>
   </si>
@@ -541,13 +541,10 @@
     <t>tester100</t>
   </si>
   <si>
-    <t>neethu111</t>
-  </si>
-  <si>
-    <t>neethu422</t>
-  </si>
-  <si>
     <t>test256</t>
+  </si>
+  <si>
+    <t>neethunew</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AC4E1D-DEF7-40CA-B4FC-DEED434DA9FE}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +1816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B889F398-F614-4537-9F12-00E692AE7DD1}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1861,7 +1858,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
         <v>162</v>
@@ -2067,7 +2064,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>

</xml_diff>